<commit_message>
Debugged teamedSampleTeachers to build teamed_4_sections.txt properly
</commit_message>
<xml_diff>
--- a/runs/constraint_files/17-18 HUMs at a glance.xlsx
+++ b/runs/constraint_files/17-18 HUMs at a glance.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SarahGold/Documents/GitHub/scheduler/runs/constraint_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21570094-9B90-2648-A67C-C25D488ECEFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="13395" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="140">
   <si>
     <t>Section ID</t>
   </si>
@@ -441,8 +447,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1260,6 +1266,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1307,7 +1316,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1340,9 +1349,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1375,6 +1401,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1550,37 +1593,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:K18"/>
+      <selection activeCell="R22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="10"/>
-    <col min="13" max="13" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="10"/>
+    <col min="13" max="13" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1609,7 +1652,7 @@
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1650,7 +1693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1693,7 +1736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -1767,7 +1810,7 @@
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
@@ -1808,7 +1851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -1851,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -1894,7 +1937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
@@ -1923,7 +1966,7 @@
       <c r="N9" s="13"/>
       <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
@@ -1952,7 +1995,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="11"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
@@ -1981,7 +2024,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
@@ -2010,7 +2053,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>19</v>
       </c>
@@ -2041,7 +2084,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="16" thickTop="1">
       <c r="A14" s="1" t="s">
         <v>112</v>
       </c>
@@ -2080,7 +2123,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="17" t="s">
         <v>113</v>
       </c>
@@ -2119,7 +2162,7 @@
       <c r="N15" s="7"/>
       <c r="O15" s="11"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="17" t="s">
         <v>114</v>
       </c>
@@ -2158,7 +2201,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="17" t="s">
         <v>115</v>
       </c>
@@ -2197,7 +2240,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="11"/>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="16" thickBot="1">
       <c r="A18" s="19" t="s">
         <v>116</v>
       </c>
@@ -2236,7 +2279,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="16" thickTop="1">
       <c r="A19" s="16" t="s">
         <v>21</v>
       </c>
@@ -2265,7 +2308,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="11"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="12" t="s">
         <v>23</v>
       </c>
@@ -2294,7 +2337,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="23"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -2311,7 +2354,7 @@
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="12" t="s">
         <v>66</v>
       </c>
@@ -2393,7 +2436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="12" t="s">
         <v>68</v>
       </c>
@@ -2434,7 +2477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="12" t="s">
         <v>69</v>
       </c>
@@ -2479,7 +2522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="12" t="s">
         <v>70</v>
       </c>
@@ -2508,7 +2551,7 @@
       <c r="N26" s="13"/>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="12" t="s">
         <v>72</v>
       </c>
@@ -2537,7 +2580,7 @@
       <c r="N27" s="7"/>
       <c r="O27" s="11"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="12" t="s">
         <v>73</v>
       </c>
@@ -2566,7 +2609,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="11"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="12" t="s">
         <v>75</v>
       </c>
@@ -2595,7 +2638,7 @@
       <c r="N29" s="7"/>
       <c r="O29" s="11"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="12" t="s">
         <v>76</v>
       </c>
@@ -2626,7 +2669,7 @@
       <c r="N30" s="7"/>
       <c r="O30" s="11"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="12" t="s">
         <v>77</v>
       </c>
@@ -2655,7 +2698,7 @@
       <c r="N31" s="7"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="12" t="s">
         <v>78</v>
       </c>
@@ -2684,7 +2727,7 @@
       <c r="N32" s="7"/>
       <c r="O32" s="11"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="12" t="s">
         <v>79</v>
       </c>
@@ -2713,7 +2756,7 @@
       <c r="N33" s="7"/>
       <c r="O33" s="11"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="12" t="s">
         <v>81</v>
       </c>
@@ -2742,7 +2785,7 @@
       <c r="N34" s="7"/>
       <c r="O34" s="11"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="12" t="s">
         <v>82</v>
       </c>
@@ -2771,7 +2814,7 @@
       <c r="N35" s="7"/>
       <c r="O35" s="11"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="12" t="s">
         <v>84</v>
       </c>
@@ -2800,7 +2843,7 @@
       <c r="N36" s="7"/>
       <c r="O36" s="11"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="12" t="s">
         <v>85</v>
       </c>
@@ -2829,7 +2872,7 @@
       <c r="N37" s="7"/>
       <c r="O37" s="11"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="12" t="s">
         <v>86</v>
       </c>
@@ -2858,7 +2901,7 @@
       <c r="N38" s="7"/>
       <c r="O38" s="11"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="12" t="s">
         <v>87</v>
       </c>
@@ -2896,21 +2939,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -2921,7 +2964,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -2932,7 +2975,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2943,7 +2986,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2954,7 +2997,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2965,7 +3008,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -2976,7 +3019,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -2987,7 +3030,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -2998,7 +3041,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -3009,7 +3052,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -3020,7 +3063,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -3031,7 +3074,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -3042,7 +3085,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -3053,7 +3096,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3064,7 +3107,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3075,7 +3118,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3086,7 +3129,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -3097,7 +3140,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -3114,13 +3157,1275 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="10"/>
+    <col min="13" max="13" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1640625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12">
+        <v>3</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="12">
+        <v>4</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="12">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="12">
+        <v>3</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="12">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12">
+        <v>3</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="12">
+        <v>4</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="12">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="12">
+        <v>3</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="12">
+        <v>6</v>
+      </c>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12">
+        <v>6</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="12">
+        <v>5</v>
+      </c>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="12">
+        <v>6</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="12">
+        <v>7</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="12">
+        <v>7</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="12">
+        <v>6</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="11"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12">
+        <v>6</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="12">
+        <v>7</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="12">
+        <v>7</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="12">
+        <v>6</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" ht="16" thickBot="1">
+      <c r="A13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="9">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="9">
+        <v>3</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" ht="16" thickTop="1">
+      <c r="A14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="14">
+        <v>4</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" s="5">
+        <v>2</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="12">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="12">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="K15" s="18">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="12">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="12">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K16" s="18">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="12">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K17" s="18">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15" ht="16" thickBot="1">
+      <c r="A18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="20">
+        <v>1</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="20">
+        <v>2</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="11"/>
+    </row>
+    <row r="19" spans="1:15" ht="16" thickTop="1">
+      <c r="A19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="16">
+        <v>3</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="16">
+        <v>4</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="11"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="12">
+        <v>4</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="12">
+        <v>3</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="23"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="12">
+        <v>2</v>
+      </c>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="12">
+        <v>2</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="12">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="12">
+        <v>4</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="12">
+        <v>7</v>
+      </c>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="12">
+        <v>1</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="12">
+        <v>2</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="8"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="12">
+        <v>2</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="12">
+        <v>1</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="12">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="12">
+        <v>2</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="11"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="12">
+        <v>2</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="12">
+        <v>1</v>
+      </c>
+      <c r="H27" s="12"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="11"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="12">
+        <v>4</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="12">
+        <v>3</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="11"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="12">
+        <v>5</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="12">
+        <v>6</v>
+      </c>
+      <c r="H29" s="12"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="11"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="12">
+        <v>6</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="12">
+        <v>5</v>
+      </c>
+      <c r="H30" s="12"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="11"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="12">
+        <v>5</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="12">
+        <v>6</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="11"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="12">
+        <v>6</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="12">
+        <v>5</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="11"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="12">
+        <v>6</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="12">
+        <v>7</v>
+      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="11"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="12">
+        <v>7</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="12">
+        <v>6</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="11"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="12">
+        <v>6</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="12">
+        <v>7</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="11"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="12">
+        <v>7</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="12">
+        <v>6</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="11"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="12">
+        <v>7</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="12">
+        <v>1</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="23"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="12">
+        <v>6</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="12">
+        <v>5</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="12">
+        <v>2</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="12">
+        <v>1</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G41" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="12">
+        <v>6</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="12">
+        <v>7</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="12">
+        <v>3</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="12">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Continued work on reading in full school sections
</commit_message>
<xml_diff>
--- a/runs/constraint_files/17-18 HUMs at a glance.xlsx
+++ b/runs/constraint_files/17-18 HUMs at a glance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SarahGold/Documents/GitHub/scheduler/runs/constraint_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21570094-9B90-2648-A67C-C25D488ECEFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B40146-AEFB-8F46-822F-DED69C165131}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3160,7 +3160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Worked on building full school sections list
</commit_message>
<xml_diff>
--- a/runs/constraint_files/17-18 HUMs at a glance.xlsx
+++ b/runs/constraint_files/17-18 HUMs at a glance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SarahGold/Documents/GitHub/scheduler/runs/constraint_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B40146-AEFB-8F46-822F-DED69C165131}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78737693-3165-1F4B-A6E6-EBFAAD66B206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="204">
   <si>
     <t>Section ID</t>
   </si>
@@ -442,6 +442,198 @@
   </si>
   <si>
     <t>Harris</t>
+  </si>
+  <si>
+    <t>1130T1-03</t>
+  </si>
+  <si>
+    <t>Glotfelty, Stephanie</t>
+  </si>
+  <si>
+    <t>1130T1-01</t>
+  </si>
+  <si>
+    <t>1130T1-02</t>
+  </si>
+  <si>
+    <t>1130T1-15</t>
+  </si>
+  <si>
+    <t>1130T1-13</t>
+  </si>
+  <si>
+    <t>1130T1-14</t>
+  </si>
+  <si>
+    <t>1130T1-09</t>
+  </si>
+  <si>
+    <t>1130T1-07</t>
+  </si>
+  <si>
+    <t>1130T1-08</t>
+  </si>
+  <si>
+    <t>Harris, Erinn</t>
+  </si>
+  <si>
+    <t>1130T1-06</t>
+  </si>
+  <si>
+    <t>1130T1-04</t>
+  </si>
+  <si>
+    <t>1130T1-05</t>
+  </si>
+  <si>
+    <t>1130T1-18</t>
+  </si>
+  <si>
+    <t>1130T1-16</t>
+  </si>
+  <si>
+    <t>1130T1-17</t>
+  </si>
+  <si>
+    <t>Lago, Natalie D.</t>
+  </si>
+  <si>
+    <t>1130T1-12</t>
+  </si>
+  <si>
+    <t>1130T1-10</t>
+  </si>
+  <si>
+    <t>1130T1-11</t>
+  </si>
+  <si>
+    <t>984060-02</t>
+  </si>
+  <si>
+    <t>984060-03</t>
+  </si>
+  <si>
+    <t>984060-11</t>
+  </si>
+  <si>
+    <t>984060-01</t>
+  </si>
+  <si>
+    <t>Geiger, Monica G.</t>
+  </si>
+  <si>
+    <t>984060-12</t>
+  </si>
+  <si>
+    <t>984060-10</t>
+  </si>
+  <si>
+    <t>Jones, Darcie</t>
+  </si>
+  <si>
+    <t>984060-05</t>
+  </si>
+  <si>
+    <t>984060-06</t>
+  </si>
+  <si>
+    <t>984060-04</t>
+  </si>
+  <si>
+    <t>984060-17</t>
+  </si>
+  <si>
+    <t>984060-18</t>
+  </si>
+  <si>
+    <t>984060-16</t>
+  </si>
+  <si>
+    <t>Seyler, Jared C.</t>
+  </si>
+  <si>
+    <t>984060-08</t>
+  </si>
+  <si>
+    <t>984060-09</t>
+  </si>
+  <si>
+    <t>984060-07</t>
+  </si>
+  <si>
+    <t>984060-14</t>
+  </si>
+  <si>
+    <t>984060-15</t>
+  </si>
+  <si>
+    <t>984060-13</t>
+  </si>
+  <si>
+    <t>Holman, Aubrie</t>
+  </si>
+  <si>
+    <t>4310T1-01</t>
+  </si>
+  <si>
+    <t>4310T1-02</t>
+  </si>
+  <si>
+    <t>4310T1-03</t>
+  </si>
+  <si>
+    <t>4310T1-10</t>
+  </si>
+  <si>
+    <t>4310T1-11</t>
+  </si>
+  <si>
+    <t>4310T1-12</t>
+  </si>
+  <si>
+    <t>James, Jennifer</t>
+  </si>
+  <si>
+    <t>4310T1-13</t>
+  </si>
+  <si>
+    <t>4310T1-14</t>
+  </si>
+  <si>
+    <t>4310T1-15</t>
+  </si>
+  <si>
+    <t>4310T1-07</t>
+  </si>
+  <si>
+    <t>4310T1-08</t>
+  </si>
+  <si>
+    <t>4310T1-09</t>
+  </si>
+  <si>
+    <t>Larson, Thomas</t>
+  </si>
+  <si>
+    <t>Rosenblum, Jennifer</t>
+  </si>
+  <si>
+    <t>4310T1-04</t>
+  </si>
+  <si>
+    <t>4310T1-05</t>
+  </si>
+  <si>
+    <t>4310T1-06</t>
+  </si>
+  <si>
+    <t>4310T1-16</t>
+  </si>
+  <si>
+    <t>4310T1-17</t>
+  </si>
+  <si>
+    <t>4310T1-18</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1333,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1215,6 +1407,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3158,10 +3351,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -3205,13 +3398,19 @@
         <v>2</v>
       </c>
       <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="I1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="12" t="s">
@@ -3234,13 +3433,13 @@
         <v>4</v>
       </c>
       <c r="H2" s="12"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="7"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="12" t="s">
@@ -3263,6 +3462,13 @@
         <v>3</v>
       </c>
       <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="7"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="12" t="s">
@@ -3287,6 +3493,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="7"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
@@ -3312,10 +3525,10 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="L5" s="7"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
@@ -3338,13 +3551,13 @@
         <v>3</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="7"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
@@ -3367,6 +3580,13 @@
         <v>6</v>
       </c>
       <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
@@ -3389,6 +3609,13 @@
         <v>5</v>
       </c>
       <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="12" t="s">
@@ -3411,13 +3638,13 @@
         <v>7</v>
       </c>
       <c r="H9" s="12"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="8"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="12" t="s">
@@ -3440,13 +3667,13 @@
         <v>6</v>
       </c>
       <c r="H10" s="12"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="11"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="12" t="s">
@@ -3469,13 +3696,13 @@
         <v>7</v>
       </c>
       <c r="H11" s="12"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="11"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="12" t="s">
@@ -3498,13 +3725,13 @@
         <v>6</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="11"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
@@ -3528,14 +3755,14 @@
       <c r="G13" s="9">
         <v>3</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="11"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
       <c r="A14" s="1" t="s">
@@ -3559,22 +3786,22 @@
       <c r="G14" s="14">
         <v>4</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="12">
         <v>2</v>
       </c>
-      <c r="L14" s="3"/>
+      <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="11"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="17" t="s">
@@ -3607,13 +3834,13 @@
       <c r="J15" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="12">
         <v>1</v>
       </c>
-      <c r="L15" s="3"/>
+      <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="11"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="17" t="s">
@@ -3646,13 +3873,13 @@
       <c r="J16" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="12">
         <v>1</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="11"/>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="17" t="s">
@@ -3685,13 +3912,13 @@
       <c r="J17" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="12">
         <v>2</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="7"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="11"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" spans="1:15" ht="16" thickBot="1">
       <c r="A18" s="19" t="s">
@@ -3715,22 +3942,22 @@
       <c r="G18" s="20">
         <v>2</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="12">
         <v>3</v>
       </c>
-      <c r="L18" s="3"/>
+      <c r="L18" s="7"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
-      <c r="O18" s="11"/>
+      <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
       <c r="A19" s="16" t="s">
@@ -3752,14 +3979,14 @@
       <c r="G19" s="16">
         <v>4</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
-      <c r="O19" s="11"/>
+      <c r="O19" s="7"/>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="12" t="s">
@@ -3781,14 +4008,14 @@
       <c r="G20" s="12">
         <v>3</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="23"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="12" t="s">
@@ -3811,6 +4038,13 @@
         <v>2</v>
       </c>
       <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="12" t="s">
@@ -3833,6 +4067,13 @@
         <v>1</v>
       </c>
       <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="12" t="s">
@@ -3857,6 +4098,13 @@
         <v>7</v>
       </c>
       <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="12" t="s">
@@ -3879,13 +4127,13 @@
         <v>2</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="8"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="12" t="s">
@@ -3908,13 +4156,13 @@
         <v>1</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
-      <c r="O25" s="11"/>
+      <c r="O25" s="7"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="12" t="s">
@@ -3937,13 +4185,13 @@
         <v>2</v>
       </c>
       <c r="H26" s="12"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
-      <c r="O26" s="11"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="12" t="s">
@@ -3966,13 +4214,13 @@
         <v>1</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
-      <c r="O27" s="11"/>
+      <c r="O27" s="7"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="12" t="s">
@@ -3997,13 +4245,13 @@
         <v>3</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="11"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="12" t="s">
@@ -4026,13 +4274,13 @@
         <v>6</v>
       </c>
       <c r="H29" s="12"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
-      <c r="O29" s="11"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="12" t="s">
@@ -4055,13 +4303,13 @@
         <v>5</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="11"/>
+      <c r="O30" s="7"/>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="12" t="s">
@@ -4084,13 +4332,13 @@
         <v>6</v>
       </c>
       <c r="H31" s="12"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
-      <c r="O31" s="11"/>
+      <c r="O31" s="7"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="12" t="s">
@@ -4113,13 +4361,13 @@
         <v>5</v>
       </c>
       <c r="H32" s="12"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
-      <c r="O32" s="11"/>
+      <c r="O32" s="7"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="12" t="s">
@@ -4142,13 +4390,13 @@
         <v>7</v>
       </c>
       <c r="H33" s="12"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
-      <c r="O33" s="11"/>
+      <c r="O33" s="7"/>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="12" t="s">
@@ -4171,13 +4419,13 @@
         <v>6</v>
       </c>
       <c r="H34" s="12"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
-      <c r="O34" s="11"/>
+      <c r="O34" s="7"/>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="12" t="s">
@@ -4200,13 +4448,13 @@
         <v>7</v>
       </c>
       <c r="H35" s="12"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
-      <c r="O35" s="11"/>
+      <c r="O35" s="7"/>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="12" t="s">
@@ -4229,13 +4477,13 @@
         <v>6</v>
       </c>
       <c r="H36" s="12"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
-      <c r="O36" s="11"/>
+      <c r="O36" s="7"/>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="12" t="s">
@@ -4260,13 +4508,13 @@
         <v>1</v>
       </c>
       <c r="H37" s="12"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="23"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="12" t="s">
@@ -4290,6 +4538,14 @@
       <c r="G38" s="12">
         <v>5</v>
       </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="12" t="s">
@@ -4313,6 +4569,14 @@
       <c r="G39" s="12">
         <v>6</v>
       </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="12" t="s">
@@ -4336,6 +4600,14 @@
       <c r="G40" s="12">
         <v>1</v>
       </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="12" t="s">
@@ -4359,6 +4631,14 @@
       <c r="G41" s="12">
         <v>2</v>
       </c>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="12" t="s">
@@ -4380,6 +4660,14 @@
       <c r="G42" s="12">
         <v>7</v>
       </c>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="12" t="s">
@@ -4401,6 +4689,14 @@
       <c r="G43" s="12">
         <v>6</v>
       </c>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="12" t="s">
@@ -4423,6 +4719,572 @@
       </c>
       <c r="G44" s="12">
         <v>4</v>
+      </c>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G45" s="12">
+        <v>2</v>
+      </c>
+      <c r="H45" s="12"/>
+      <c r="I45" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K45" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="12">
+        <v>2</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G46" s="12">
+        <v>3</v>
+      </c>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K46" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="12">
+        <v>3</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G47" s="12">
+        <v>1</v>
+      </c>
+      <c r="H47" s="12"/>
+      <c r="I47" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K47" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="12">
+        <v>5</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G48" s="12">
+        <v>6</v>
+      </c>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="K48" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="12">
+        <v>6</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" s="12">
+        <v>7</v>
+      </c>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="K49" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="12">
+        <v>7</v>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G50" s="12">
+        <v>5</v>
+      </c>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="K50" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="12">
+        <v>1</v>
+      </c>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G51" s="12">
+        <v>2</v>
+      </c>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="K51" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="12">
+        <v>2</v>
+      </c>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G52" s="12">
+        <v>3</v>
+      </c>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="K52" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" s="12">
+        <v>3</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G53" s="12">
+        <v>1</v>
+      </c>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="J53" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="K53" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="12">
+        <v>1</v>
+      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" s="12">
+        <v>2</v>
+      </c>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="K54" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="12">
+        <v>2</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G55" s="12">
+        <v>3</v>
+      </c>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="K55" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="12">
+        <v>3</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G56" s="12">
+        <v>1</v>
+      </c>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="K56" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="12">
+        <v>5</v>
+      </c>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G57" s="12">
+        <v>6</v>
+      </c>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="J57" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="K57" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" s="12">
+        <v>6</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G58" s="12">
+        <v>7</v>
+      </c>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="K58" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" s="12">
+        <v>7</v>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59" s="12">
+        <v>5</v>
+      </c>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="K59" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C60" s="12">
+        <v>5</v>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G60" s="12">
+        <v>6</v>
+      </c>
+      <c r="H60" s="12"/>
+      <c r="I60" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="J60" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K60" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="12">
+        <v>6</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G61" s="12">
+        <v>7</v>
+      </c>
+      <c r="H61" s="12"/>
+      <c r="I61" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K61" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" s="12">
+        <v>7</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G62" s="12">
+        <v>5</v>
+      </c>
+      <c r="H62" s="12"/>
+      <c r="I62" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="J62" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K62" s="12">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added team_3 to teamedSampleTeachers.py and contineued work on full_school_sections.py
</commit_message>
<xml_diff>
--- a/runs/constraint_files/17-18 HUMs at a glance.xlsx
+++ b/runs/constraint_files/17-18 HUMs at a glance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SarahGold/Documents/GitHub/scheduler/runs/constraint_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78737693-3165-1F4B-A6E6-EBFAAD66B206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB5E130-04AD-9B4F-A849-6A68954EFCFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="205">
   <si>
     <t>Section ID</t>
   </si>
@@ -634,6 +635,9 @@
   </si>
   <si>
     <t>4310T1-18</t>
+  </si>
+  <si>
+    <t>IBET</t>
   </si>
 </sst>
 </file>
@@ -3353,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -4526,9 +4530,7 @@
       <c r="C38" s="12">
         <v>6</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>102</v>
-      </c>
+      <c r="D38" s="12"/>
       <c r="E38" s="12" t="s">
         <v>97</v>
       </c>
@@ -4557,9 +4559,7 @@
       <c r="C39" s="12">
         <v>5</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>102</v>
-      </c>
+      <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
         <v>99</v>
       </c>
@@ -4588,9 +4588,7 @@
       <c r="C40" s="12">
         <v>2</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>103</v>
-      </c>
+      <c r="D40" s="12"/>
       <c r="E40" s="12" t="s">
         <v>107</v>
       </c>
@@ -4619,9 +4617,7 @@
       <c r="C41" s="12">
         <v>1</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>103</v>
-      </c>
+      <c r="D41" s="12"/>
       <c r="E41" s="12" t="s">
         <v>108</v>
       </c>
@@ -4739,7 +4735,9 @@
       <c r="C45" s="12">
         <v>1</v>
       </c>
-      <c r="D45" s="12"/>
+      <c r="D45" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E45" s="12" t="s">
         <v>162</v>
       </c>
@@ -4749,7 +4747,9 @@
       <c r="G45" s="12">
         <v>2</v>
       </c>
-      <c r="H45" s="12"/>
+      <c r="H45" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I45" s="25" t="s">
         <v>185</v>
       </c>
@@ -4770,7 +4770,9 @@
       <c r="C46" s="12">
         <v>2</v>
       </c>
-      <c r="D46" s="12"/>
+      <c r="D46" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E46" s="12" t="s">
         <v>164</v>
       </c>
@@ -4780,7 +4782,9 @@
       <c r="G46" s="12">
         <v>3</v>
       </c>
-      <c r="H46" s="12"/>
+      <c r="H46" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I46" s="12" t="s">
         <v>183</v>
       </c>
@@ -4801,7 +4805,9 @@
       <c r="C47" s="12">
         <v>3</v>
       </c>
-      <c r="D47" s="12"/>
+      <c r="D47" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E47" s="12" t="s">
         <v>161</v>
       </c>
@@ -4811,7 +4817,9 @@
       <c r="G47" s="12">
         <v>1</v>
       </c>
-      <c r="H47" s="12"/>
+      <c r="H47" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I47" s="25" t="s">
         <v>184</v>
       </c>
@@ -4832,7 +4840,9 @@
       <c r="C48" s="12">
         <v>5</v>
       </c>
-      <c r="D48" s="12"/>
+      <c r="D48" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E48" s="12" t="s">
         <v>180</v>
       </c>
@@ -4842,7 +4852,9 @@
       <c r="G48" s="12">
         <v>6</v>
       </c>
-      <c r="H48" s="12"/>
+      <c r="H48" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I48" s="12" t="s">
         <v>192</v>
       </c>
@@ -4863,7 +4875,9 @@
       <c r="C49" s="12">
         <v>6</v>
       </c>
-      <c r="D49" s="12"/>
+      <c r="D49" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E49" s="12" t="s">
         <v>181</v>
       </c>
@@ -4873,7 +4887,9 @@
       <c r="G49" s="12">
         <v>7</v>
       </c>
-      <c r="H49" s="12"/>
+      <c r="H49" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I49" s="12" t="s">
         <v>190</v>
       </c>
@@ -4894,7 +4910,9 @@
       <c r="C50" s="12">
         <v>7</v>
       </c>
-      <c r="D50" s="12"/>
+      <c r="D50" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E50" s="12" t="s">
         <v>179</v>
       </c>
@@ -4904,7 +4922,9 @@
       <c r="G50" s="12">
         <v>5</v>
       </c>
-      <c r="H50" s="12"/>
+      <c r="H50" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I50" s="12" t="s">
         <v>191</v>
       </c>
@@ -4925,7 +4945,9 @@
       <c r="C51" s="12">
         <v>1</v>
       </c>
-      <c r="D51" s="12"/>
+      <c r="D51" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E51" s="12" t="s">
         <v>177</v>
       </c>
@@ -4935,7 +4957,9 @@
       <c r="G51" s="12">
         <v>2</v>
       </c>
-      <c r="H51" s="12"/>
+      <c r="H51" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I51" s="12" t="s">
         <v>195</v>
       </c>
@@ -4956,7 +4980,9 @@
       <c r="C52" s="12">
         <v>2</v>
       </c>
-      <c r="D52" s="12"/>
+      <c r="D52" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E52" s="12" t="s">
         <v>178</v>
       </c>
@@ -4966,7 +4992,9 @@
       <c r="G52" s="12">
         <v>3</v>
       </c>
-      <c r="H52" s="12"/>
+      <c r="H52" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I52" s="12" t="s">
         <v>193</v>
       </c>
@@ -4987,7 +5015,9 @@
       <c r="C53" s="12">
         <v>3</v>
       </c>
-      <c r="D53" s="12"/>
+      <c r="D53" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E53" s="12" t="s">
         <v>176</v>
       </c>
@@ -4997,7 +5027,9 @@
       <c r="G53" s="12">
         <v>1</v>
       </c>
-      <c r="H53" s="12"/>
+      <c r="H53" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I53" s="12" t="s">
         <v>194</v>
       </c>
@@ -5018,7 +5050,9 @@
       <c r="C54" s="12">
         <v>1</v>
       </c>
-      <c r="D54" s="12"/>
+      <c r="D54" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E54" s="12" t="s">
         <v>170</v>
       </c>
@@ -5028,7 +5062,9 @@
       <c r="G54" s="12">
         <v>2</v>
       </c>
-      <c r="H54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I54" s="12" t="s">
         <v>200</v>
       </c>
@@ -5049,7 +5085,9 @@
       <c r="C55" s="12">
         <v>2</v>
       </c>
-      <c r="D55" s="12"/>
+      <c r="D55" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E55" s="12" t="s">
         <v>171</v>
       </c>
@@ -5059,7 +5097,9 @@
       <c r="G55" s="12">
         <v>3</v>
       </c>
-      <c r="H55" s="12"/>
+      <c r="H55" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I55" s="12" t="s">
         <v>198</v>
       </c>
@@ -5080,7 +5120,9 @@
       <c r="C56" s="12">
         <v>3</v>
       </c>
-      <c r="D56" s="12"/>
+      <c r="D56" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E56" s="12" t="s">
         <v>169</v>
       </c>
@@ -5090,7 +5132,9 @@
       <c r="G56" s="12">
         <v>1</v>
       </c>
-      <c r="H56" s="12"/>
+      <c r="H56" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I56" s="12" t="s">
         <v>199</v>
       </c>
@@ -5111,7 +5155,9 @@
       <c r="C57" s="12">
         <v>5</v>
       </c>
-      <c r="D57" s="12"/>
+      <c r="D57" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E57" s="12" t="s">
         <v>173</v>
       </c>
@@ -5121,7 +5167,9 @@
       <c r="G57" s="12">
         <v>6</v>
       </c>
-      <c r="H57" s="12"/>
+      <c r="H57" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I57" s="12" t="s">
         <v>203</v>
       </c>
@@ -5142,7 +5190,9 @@
       <c r="C58" s="12">
         <v>6</v>
       </c>
-      <c r="D58" s="12"/>
+      <c r="D58" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E58" s="12" t="s">
         <v>174</v>
       </c>
@@ -5152,7 +5202,9 @@
       <c r="G58" s="12">
         <v>7</v>
       </c>
-      <c r="H58" s="12"/>
+      <c r="H58" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I58" s="12" t="s">
         <v>201</v>
       </c>
@@ -5173,7 +5225,9 @@
       <c r="C59" s="12">
         <v>7</v>
       </c>
-      <c r="D59" s="12"/>
+      <c r="D59" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E59" s="12" t="s">
         <v>172</v>
       </c>
@@ -5183,7 +5237,9 @@
       <c r="G59" s="12">
         <v>5</v>
       </c>
-      <c r="H59" s="12"/>
+      <c r="H59" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I59" s="12" t="s">
         <v>202</v>
       </c>
@@ -5204,7 +5260,9 @@
       <c r="C60" s="12">
         <v>5</v>
       </c>
-      <c r="D60" s="12"/>
+      <c r="D60" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E60" s="12" t="s">
         <v>166</v>
       </c>
@@ -5214,7 +5272,9 @@
       <c r="G60" s="12">
         <v>6</v>
       </c>
-      <c r="H60" s="12"/>
+      <c r="H60" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I60" s="25" t="s">
         <v>188</v>
       </c>
@@ -5235,7 +5295,9 @@
       <c r="C61" s="12">
         <v>6</v>
       </c>
-      <c r="D61" s="12"/>
+      <c r="D61" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E61" s="12" t="s">
         <v>167</v>
       </c>
@@ -5245,7 +5307,9 @@
       <c r="G61" s="12">
         <v>7</v>
       </c>
-      <c r="H61" s="12"/>
+      <c r="H61" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I61" s="25" t="s">
         <v>186</v>
       </c>
@@ -5266,7 +5330,9 @@
       <c r="C62" s="12">
         <v>7</v>
       </c>
-      <c r="D62" s="12"/>
+      <c r="D62" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E62" s="12" t="s">
         <v>163</v>
       </c>
@@ -5276,7 +5342,9 @@
       <c r="G62" s="12">
         <v>5</v>
       </c>
-      <c r="H62" s="12"/>
+      <c r="H62" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="I62" s="25" t="s">
         <v>187</v>
       </c>

</xml_diff>